<commit_message>
Worked for the Yolo model part to create one complete framework from prediction to generate metrics. It is completed.
</commit_message>
<xml_diff>
--- a/modules/metrics/yolo_pred_labels_normalized.xlsx
+++ b/modules/metrics/yolo_pred_labels_normalized.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Oslo\OsloMet\Fourth semester\DetectionOfBallotPaper\modules\ai_detection_model\src\model\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Oslo\OsloMet\Fourth semester\DetectionOfBallotPaper\modules\metrics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47A3F884-7C81-445A-B6E4-3081D6D3064C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65EDFEB7-B2A6-4A3E-B297-D38D9B8C7D08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="34035" yWindow="3285" windowWidth="21600" windowHeight="12585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -841,6 +841,7 @@
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="8" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">

</xml_diff>